<commit_message>
produced argument level figures
</commit_message>
<xml_diff>
--- a/MSci Results Table.xlsx
+++ b/MSci Results Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayangzhang/Library/CloudStorage/GoogleDrive-jiayang.zhang@icloud.com/My Drive/Imperial/nlp-physicseducation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4EAC2-2B95-5A4F-92ED-90C0FAD7772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46622693-38AB-CF4B-B145-D1C72D752E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="21960" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{26A7B5C3-2A23-2942-801D-710FEB5E2E5F}"/>
+    <workbookView xWindow="20680" yWindow="500" windowWidth="15480" windowHeight="17440" xr2:uid="{26A7B5C3-2A23-2942-801D-710FEB5E2E5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>Year</t>
   </si>
@@ -62,16 +62,7 @@
     <t>ReasoningLevel</t>
   </si>
   <si>
-    <t>BERT-accy</t>
-  </si>
-  <si>
     <t>[0.2, 0.3, 0.4, 0.5, 0.6, 0.7, 0.8, 0.9]</t>
-  </si>
-  <si>
-    <t>[0.47222221493721006, 0.459375, 0.45178571343421936, 0.5041666686534881, 0.49750000834465025, 0.75, 0.6208333432674408, 0.825]</t>
-  </si>
-  <si>
-    <t>[0.008784104088006155, 0.01384378527083543, 0.00919252600184733, 0.04161455118809117, 0.026634096005599506, 0.028384222069663984, 0.08421409751357443, 0.03775951866748304]</t>
   </si>
   <si>
     <t>ArgumentLevel</t>
@@ -84,14 +75,122 @@
     <t>[0.043645155324258236, 0.010186253758129139, 0.01988487475075547, 0.011410886614691999, 0.02604083366333376, 0.038590903235088965, 0.030900831717867647, 0.04026280852101601]</t>
   </si>
   <si>
-    <t>BERT-loss</t>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>[0.37249999940395356, 0.3875, 0.428125, 0.44166666865348814, 0.45416665971279147, 0.425, 0.5375, 0.6375]</t>
+  </si>
+  <si>
+    <t>[0.0636641563932575, 0.03791437692549185, 0.021875, 0.02019866648241811, 0.060164700158199594, 0.03903123748998998, 0.0375, 0.04592793267718459]</t>
+  </si>
+  <si>
+    <t>BERT</t>
+  </si>
+  <si>
+    <t>training loss error</t>
+  </si>
+  <si>
+    <t>training loss</t>
+  </si>
+  <si>
+    <t>validation loss</t>
+  </si>
+  <si>
+    <t>validation loss error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.5689340353012085, 1.5278773307800293, 1.40837721824646, 1.3456363916397094, 1.4132815599441528, 1.2430763244628906, 1.1133771419525147, 0.9068126797676086] </t>
+  </si>
+  <si>
+    <t>[0.0596535666182944, 0.07256015824850842, 0.026598958986523157, 0.01306054012041525, 0.12170919950311919, 0.013109738227438637, 0.023957583858014612, 0.03108869314011349]</t>
+  </si>
+  <si>
+    <t>[0.0855829523007031, 0.05654021143720881, 0.014394939639242165, 0.0348266581982038, 0.10428498015438234, 0.04776953733077656, 0.025651201878988214, 0.03777506040937853]</t>
+  </si>
+  <si>
+    <t>[1.5145948648452758, 1.4736609935760498, 1.3669594049453735, 1.3064099311828614, 1.3074922561645508, 1.2479949951171876, 1.072635006904602, 0.9240402460098267]</t>
+  </si>
+  <si>
+    <t>[0.5399999916553497, 0.36749999821186063, 0.53125, 0.5583333253860474, 0.5875000119209289, 0.5125, 0.55, 0.5375]</t>
+  </si>
+  <si>
+    <t>[0.022150052968742426, 0.08879400169070821, 0.02209708691207961, 0.0190940692976895, 0.029755947195119415, 0.02898005779842407, 0.03365728004459065, 0.03186887195995491]</t>
+  </si>
+  <si>
+    <t>[1.0846369862556458, 1.252258014678955, 1.0770849347114564, 1.0623918533325196, 1.078547513484955, 1.0799781799316406, 1.0658930659294128, 1.0462480783462524]</t>
+  </si>
+  <si>
+    <t>[0.04605338463339965, 0.11634846688263102, 0.05890664389597926, 0.030456801335815995, 0.039498232252787556, 0.03019442389711069, 0.020053604811313762, 0.008261640304774342]</t>
+  </si>
+  <si>
+    <t>[1.1142802238464355, 1.2566216945648194, 1.1017011165618897, 1.0379038333892823, 1.0161292791366576, 1.066232144832611, 1.0995341062545776, 1.041537308692932]</t>
+  </si>
+  <si>
+    <t>[0.02760086402271873, 0.08289508028698087, 0.03331279488486714, 0.033657134804782954, 0.030822664891511975, 0.018692063108636938, 0.03991565109393979, 0.042230434767447755]</t>
+  </si>
+  <si>
+    <t>[1.4642749309539795, 1.4545567512512207, 1.3625159740447998, 1.3982894897460938, 1.348232913017273, 1.1222812414169312, 0.7201834321022034, 0.4796086311340332]</t>
+  </si>
+  <si>
+    <t>[0.03472154057237007, 0.04077450508696644, 0.03522157623347356, 0.03961426768881522, 0.011476712639020278, 0.05353810234357083, 0.06512447560184652, 0.04421245173818535]</t>
+  </si>
+  <si>
+    <t>[1.4745788335800172, 1.4561055183410645, 1.374446702003479, 1.401372766494751, 1.3554801940917969, 1.004001832008362, 0.5756299674510956, 0.3924282431602478]</t>
+  </si>
+  <si>
+    <t>[0.0389543777091745, 0.02636241967298983, 0.022030578008929862, 0.014185803561205313, 0.04768599087698454, 0.06684474283180379, 0.04814373669621662, 0.0945521708271562]</t>
+  </si>
+  <si>
+    <t>[0.25625, 0.275, 0.33333333432674406, 0.27916666194796563, 0.45, 0.5875, 0.625, 0.6875]</t>
+  </si>
+  <si>
+    <t>[0.04931166824393594, 0.04352621336620038, 0.04796193535417738, 0.07811805221009072, 0.055551215108222425, 0.018221724671391562, 0.01976423537605237, 0.02795084971874737]</t>
+  </si>
+  <si>
+    <t>[1.5721015453338623, 1.609110426902771, 1.5366835355758668, 1.5701447248458862, 1.4230413675308227, 1.4282742023468018, 1.18533034324646, 1.0718866348266602]</t>
+  </si>
+  <si>
+    <t>[0.10051023823437834, 0.031967806539777224, 0.04779583193301058, 0.03758434637077265, 0.027433601750596216, 0.04725804595336699, 0.02499533407945339, 0.03204971687081029]</t>
+  </si>
+  <si>
+    <t>[1.5839020013809204, 1.5545708179473876, 1.5054286241531372, 1.5591875553131103, 1.3719195604324341, 1.2997063159942628, 1.1222557067871093, 0.9939069986343384]</t>
+  </si>
+  <si>
+    <t>[0.06713586818831711, 0.04482375516893548, 0.03471429699835942, 0.03934282324939294, 0.022567933666091288, 0.03790497443498799, 0.06426581637864985, 0.05386996017665011]</t>
+  </si>
+  <si>
+    <t>[0.35, 0.378125, 0.4499999940395355, 0.4791666567325592, 0.425, 0.575, 0.625, 0.75]</t>
+  </si>
+  <si>
+    <t>[0.023489525591207667, 0.018087245160609725, 0.02243818245354381, 0.022821767788247176, 0.036443449342783124, 0.08361930100162282, 0.0739509972887452, 0.02795084971874737]</t>
+  </si>
+  <si>
+    <t>[1.3475236654281617, 1.3177565336227417, 1.2445393562316895, 1.2701226472854614, 1.2891224145889282, 1.1544225096702576, 1.131305992603302, 0.929024052619934]</t>
+  </si>
+  <si>
+    <t>[0.06409717680841215, 0.007536642252970959, 0.03317415809138291, 0.05836759924637006, 0.028693645767962458, 0.052437733591084335, 0.05421716789293246, 0.06179834533305722]</t>
+  </si>
+  <si>
+    <t>[1.3555550813674926, 1.3382904052734375, 1.210301446914673, 1.2674599885940552, 1.2752461433410645, 1.0631118297576905, 1.0617867827415466, 0.7942333817481995]</t>
+  </si>
+  <si>
+    <t>[0.028687466274809767, 0.011649073062630001, 0.02080439052358861, 0.010606464832327241, 0.01513590847480945, 0.06799731375210825, 0.1203204356388297, 0.044439330970457915]</t>
+  </si>
+  <si>
+    <t>[0.4291666686534882, 0.45625, 0.4625, 0.4541666626930237, 0.4424999952316284, 0.621875, 0.7958333373069764, 0.81875]</t>
+  </si>
+  <si>
+    <t>[0.03139626351831777, 0.018087245160609725, 0.008183174135549802, 0.013420938178366754, 0.02839453564144166, 0.05916905071487965, 0.021245915419266726, 0.03336586953759785]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,13 +204,45 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF383A42"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,12 +257,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,40 +584,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA1F9C4-D675-CE4F-A167-3A9CFB7BB95F}">
-  <dimension ref="A1:AC1000"/>
+  <dimension ref="A1:AC996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
     <col min="4" max="6" width="31.83203125" customWidth="1"/>
+    <col min="7" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -501,28 +650,36 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
+      <c r="G2" s="3" t="s">
+        <v>27</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -544,28 +701,36 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="4" t="s">
+        <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+      <c r="F3" s="3" t="s">
+        <v>42</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
+      <c r="G3" s="3" t="s">
+        <v>43</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -587,24 +752,36 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -625,87 +802,139 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:29" s="9" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+    </row>
+    <row r="6" spans="1:29" s="9" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+    </row>
+    <row r="7" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-    </row>
-    <row r="6" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-    </row>
-    <row r="7" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -31385,131 +31614,8 @@
       <c r="AB996" s="1"/>
       <c r="AC996" s="1"/>
     </row>
-    <row r="997" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="1"/>
-      <c r="B997" s="1"/>
-      <c r="C997" s="1"/>
-      <c r="D997" s="1"/>
-      <c r="E997" s="1"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-      <c r="T997" s="1"/>
-      <c r="U997" s="1"/>
-      <c r="V997" s="1"/>
-      <c r="W997" s="1"/>
-      <c r="X997" s="1"/>
-      <c r="Y997" s="1"/>
-      <c r="Z997" s="1"/>
-      <c r="AA997" s="1"/>
-      <c r="AB997" s="1"/>
-      <c r="AC997" s="1"/>
-    </row>
-    <row r="998" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-      <c r="AA998" s="1"/>
-      <c r="AB998" s="1"/>
-      <c r="AC998" s="1"/>
-    </row>
-    <row r="999" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="1"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="1"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="1"/>
-      <c r="K999" s="1"/>
-      <c r="L999" s="1"/>
-      <c r="M999" s="1"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-      <c r="AA999" s="1"/>
-      <c r="AB999" s="1"/>
-      <c r="AC999" s="1"/>
-    </row>
-    <row r="1000" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
-      <c r="AA1000" s="1"/>
-      <c r="AB1000" s="1"/>
-      <c r="AC1000" s="1"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>